<commit_message>
added urls and loading them
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/lorenzo_lazzari6_studio_unibo_it/Documents/dash-profesion-data-es/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{F44EBF45-C205-4C15-8477-6686C66FBB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55911267-83E5-447F-8069-E0AAC45E984E}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="14_{4BB39B8D-1D79-4438-9E60-67AA297A40B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E717137-AC83-4989-8785-4738CB4B48CE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="urls" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Espana</t>
   </si>
@@ -47,18 +47,12 @@
     <t>Madrid</t>
   </si>
   <si>
-    <t>Valencia</t>
-  </si>
-  <si>
     <t>Data Engineer</t>
   </si>
   <si>
     <t>Data Scientist</t>
   </si>
   <si>
-    <t>Data Analysts</t>
-  </si>
-  <si>
     <t>Business Analyst</t>
   </si>
   <si>
@@ -74,7 +68,34 @@
     <t>https://www.glassdoor.com/Job/spain-business-analyst-jobs-SRCH_IL.0,5_IN219_KO6,22.htm?clickSource=searchBox</t>
   </si>
   <si>
+    <t>https://www.glassdoor.com/Job/barcelona-data-engineer-jobs-SRCH_IL.0,9_IC2547194_KO10,23.htm?clickSource=searchBox</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Job/madrid-data-engineer-jobs-SRCH_IL.0,6_IC2664239_KO7,20.htm?clickSource=searchBox</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Job/barcelona-data-scientist-jobs-SRCH_IL.0,9_IC2547194_KO10,24.htm?clickSource=searchBox</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Job/madrid-data-scientist-jobs-SRCH_IL.0,6_IC2664239_KO7,21.htm?clickSource=searchBox</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Job/barcelona-data-analyst-jobs-SRCH_IL.0,9_IC2547194_KO10,22.htm?clickSource=searchBox</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Job/madrid-data-analyst-jobs-SRCH_IL.0,6_IC2664239_KO7,19.htm?clickSource=searchBox</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Job/barcelona-business-analyst-jobs-SRCH_IL.0,9_IC2547194_KO10,26.htm?clickSource=searchBox</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Job/madrid-business-analyst-jobs-SRCH_IL.0,6_IC2664239_KO7,23.htm?clickSource=searchBox</t>
+  </si>
+  <si>
     <t>Area</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
   </si>
 </sst>
 </file>
@@ -437,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -450,73 +471,85 @@
     <col min="5" max="5" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
         <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{52E82E1C-B165-4D34-B094-18197D7294C2}"/>
+    <hyperlink ref="B3" r:id="rId6" xr:uid="{832D381C-A1FC-48EA-AC5A-305FCED22EC5}"/>
+    <hyperlink ref="C3" r:id="rId7" xr:uid="{C82943C8-D7BF-4C58-8104-AD3AFD65208D}"/>
+    <hyperlink ref="C4" r:id="rId8" xr:uid="{42DBDDDB-29C0-4D15-AC6F-6196C5E017BF}"/>
+    <hyperlink ref="D3" r:id="rId9" xr:uid="{37FE4113-3F20-42A3-A97F-0E314FADE934}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finally define main function in init
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/lorenzo_lazzari6_studio_unibo_it/Documents/dash-profesion-data-es/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="14_{4BB39B8D-1D79-4438-9E60-67AA297A40B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E717137-AC83-4989-8785-4738CB4B48CE}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="14_{4BB39B8D-1D79-4438-9E60-67AA297A40B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{528F2A0D-C2C4-4B46-85AF-4991B6A3C0CA}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="urls" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>Espana</t>
-  </si>
-  <si>
     <t>Barcelona</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>España</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -473,70 +473,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>